<commit_message>
Add income statement aggregation logic
Implements Stage 5b for income statement aggregation in both the notebook and script. Adds functions to normalize columns, calculate amounts by rule type, and aggregate leaf trial balances into structured income statement lines with traceable accounts. Displays the first 10 lines of the aggregated income statement if rules are provided.
</commit_message>
<xml_diff>
--- a/data/TB_2025.xlsx
+++ b/data/TB_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52ebbb93f357813a/10_Works/GitHub/Planning_Agent_NDD/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{D6582138-62CA-44CD-9C34-C9ABEF85A640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B347512-F120-42A2-8AB4-2CEC12160956}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{D6582138-62CA-44CD-9C34-C9ABEF85A640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD5C88D9-1732-4228-8276-594068816A1C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5925778F-D371-4578-87A7-1EA07C6739EF}"/>
   </bookViews>
@@ -1246,10 +1246,10 @@
   <dimension ref="A1:M135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B115" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I43" sqref="I43"/>
+      <selection pane="bottomRight" activeCell="F76" sqref="F76:G134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,7 +1258,8 @@
     <col min="2" max="2" width="37.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -4140,9 +4141,11 @@
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
+      <c r="F76" s="2">
+        <v>0</v>
+      </c>
       <c r="G76" s="2">
-        <v>0</v>
+        <v>11320490154</v>
       </c>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
@@ -4171,7 +4174,9 @@
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
+      <c r="F77" s="2">
+        <v>0</v>
+      </c>
       <c r="G77" s="2">
         <v>9761488800</v>
       </c>
@@ -4202,7 +4207,9 @@
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
-      <c r="F78" s="2"/>
+      <c r="F78" s="2">
+        <v>0</v>
+      </c>
       <c r="G78" s="2">
         <v>238844934</v>
       </c>
@@ -4233,7 +4240,9 @@
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
+      <c r="F79" s="2">
+        <v>0</v>
+      </c>
       <c r="G79" s="2">
         <v>1320156420</v>
       </c>
@@ -4264,7 +4273,9 @@
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
+      <c r="F80" s="2">
+        <v>0</v>
+      </c>
       <c r="G80" s="2">
         <v>0</v>
       </c>
@@ -4295,7 +4306,9 @@
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
+      <c r="F81" s="2">
+        <v>0</v>
+      </c>
       <c r="G81" s="2">
         <v>907591</v>
       </c>
@@ -4326,7 +4339,9 @@
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
+      <c r="F82" s="2">
+        <v>0</v>
+      </c>
       <c r="G82" s="2">
         <v>199741089</v>
       </c>
@@ -4357,7 +4372,9 @@
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
-      <c r="F83" s="2"/>
+      <c r="F83" s="2">
+        <v>0</v>
+      </c>
       <c r="G83" s="2">
         <v>42738013</v>
       </c>
@@ -4391,7 +4408,9 @@
       <c r="F84" s="2">
         <v>0</v>
       </c>
-      <c r="G84" s="2"/>
+      <c r="G84" s="2">
+        <v>0</v>
+      </c>
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
       <c r="J84">
@@ -4422,7 +4441,9 @@
       <c r="F85" s="2">
         <v>8209584118</v>
       </c>
-      <c r="G85" s="2"/>
+      <c r="G85" s="2">
+        <v>0</v>
+      </c>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
       <c r="J85">
@@ -4453,7 +4474,9 @@
       <c r="F86" s="2">
         <v>1209043426</v>
       </c>
-      <c r="G86" s="2"/>
+      <c r="G86" s="2">
+        <v>0</v>
+      </c>
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
       <c r="J86">
@@ -4484,7 +4507,9 @@
       <c r="F87" s="2">
         <v>0</v>
       </c>
-      <c r="G87" s="2"/>
+      <c r="G87" s="2">
+        <v>0</v>
+      </c>
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
       <c r="J87">
@@ -4515,7 +4540,9 @@
       <c r="F88" s="2">
         <v>62044912</v>
       </c>
-      <c r="G88" s="2"/>
+      <c r="G88" s="2">
+        <v>0</v>
+      </c>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
       <c r="J88">
@@ -4546,7 +4573,9 @@
       <c r="F89" s="2">
         <v>0</v>
       </c>
-      <c r="G89" s="2"/>
+      <c r="G89" s="2">
+        <v>0</v>
+      </c>
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
       <c r="J89">
@@ -4577,7 +4606,9 @@
       <c r="F90" s="2">
         <v>0</v>
       </c>
-      <c r="G90" s="2"/>
+      <c r="G90" s="2">
+        <v>0</v>
+      </c>
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
       <c r="J90">
@@ -4608,7 +4639,9 @@
       <c r="F91" s="2">
         <v>433406484</v>
       </c>
-      <c r="G91" s="2"/>
+      <c r="G91" s="2">
+        <v>0</v>
+      </c>
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
       <c r="J91">
@@ -4639,7 +4672,9 @@
       <c r="F92" s="2">
         <v>-725841475</v>
       </c>
-      <c r="G92" s="2"/>
+      <c r="G92" s="2">
+        <v>0</v>
+      </c>
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
       <c r="J92">
@@ -4670,7 +4705,9 @@
       <c r="F93" s="2">
         <v>78329673</v>
       </c>
-      <c r="G93" s="2"/>
+      <c r="G93" s="2">
+        <v>0</v>
+      </c>
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
       <c r="J93">
@@ -4701,7 +4738,9 @@
       <c r="F94" s="2">
         <v>362570806</v>
       </c>
-      <c r="G94" s="2"/>
+      <c r="G94" s="2">
+        <v>0</v>
+      </c>
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
       <c r="J94">
@@ -4732,7 +4771,9 @@
       <c r="F95" s="2">
         <v>815277317</v>
       </c>
-      <c r="G95" s="2"/>
+      <c r="G95" s="2">
+        <v>0</v>
+      </c>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
       <c r="J95">
@@ -4763,7 +4804,9 @@
       <c r="F96" s="2">
         <v>61558431</v>
       </c>
-      <c r="G96" s="2"/>
+      <c r="G96" s="2">
+        <v>0</v>
+      </c>
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
       <c r="J96">
@@ -4794,7 +4837,9 @@
       <c r="F97" s="2">
         <v>106263049</v>
       </c>
-      <c r="G97" s="2"/>
+      <c r="G97" s="2">
+        <v>0</v>
+      </c>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
       <c r="J97">
@@ -4825,7 +4870,9 @@
       <c r="F98" s="2">
         <v>0</v>
       </c>
-      <c r="G98" s="2"/>
+      <c r="G98" s="2">
+        <v>0</v>
+      </c>
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
       <c r="J98">
@@ -4856,7 +4903,9 @@
       <c r="F99" s="2">
         <v>4914996</v>
       </c>
-      <c r="G99" s="2"/>
+      <c r="G99" s="2">
+        <v>0</v>
+      </c>
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
       <c r="J99">
@@ -4887,7 +4936,9 @@
       <c r="F100" s="2">
         <v>0</v>
       </c>
-      <c r="G100" s="2"/>
+      <c r="G100" s="2">
+        <v>0</v>
+      </c>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
       <c r="J100">
@@ -4918,7 +4969,9 @@
       <c r="F101" s="2">
         <v>165928141</v>
       </c>
-      <c r="G101" s="2"/>
+      <c r="G101" s="2">
+        <v>0</v>
+      </c>
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
       <c r="J101">
@@ -4949,7 +5002,9 @@
       <c r="F102" s="2">
         <v>136205867</v>
       </c>
-      <c r="G102" s="2"/>
+      <c r="G102" s="2">
+        <v>0</v>
+      </c>
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
       <c r="J102">
@@ -4980,7 +5035,9 @@
       <c r="F103" s="2">
         <v>200642454</v>
       </c>
-      <c r="G103" s="2"/>
+      <c r="G103" s="2">
+        <v>0</v>
+      </c>
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
       <c r="J103">
@@ -5011,7 +5068,9 @@
       <c r="F104" s="2">
         <v>5546036</v>
       </c>
-      <c r="G104" s="2"/>
+      <c r="G104" s="2">
+        <v>0</v>
+      </c>
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
       <c r="J104">
@@ -5042,7 +5101,9 @@
       <c r="F105" s="2">
         <v>7740016</v>
       </c>
-      <c r="G105" s="2"/>
+      <c r="G105" s="2">
+        <v>0</v>
+      </c>
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
       <c r="J105">
@@ -5073,7 +5134,9 @@
       <c r="F106" s="2">
         <v>126194631</v>
       </c>
-      <c r="G106" s="2"/>
+      <c r="G106" s="2">
+        <v>0</v>
+      </c>
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
       <c r="J106">
@@ -5104,7 +5167,9 @@
       <c r="F107" s="2">
         <v>20000</v>
       </c>
-      <c r="G107" s="2"/>
+      <c r="G107" s="2">
+        <v>0</v>
+      </c>
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
       <c r="J107">
@@ -5135,7 +5200,9 @@
       <c r="F108" s="2">
         <v>0</v>
       </c>
-      <c r="G108" s="2"/>
+      <c r="G108" s="2">
+        <v>0</v>
+      </c>
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
       <c r="J108">
@@ -5166,7 +5233,9 @@
       <c r="F109" s="2">
         <v>25479000</v>
       </c>
-      <c r="G109" s="2"/>
+      <c r="G109" s="2">
+        <v>0</v>
+      </c>
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
       <c r="J109">
@@ -5197,7 +5266,9 @@
       <c r="F110" s="2">
         <v>54617294</v>
       </c>
-      <c r="G110" s="2"/>
+      <c r="G110" s="2">
+        <v>0</v>
+      </c>
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
       <c r="J110">
@@ -5228,7 +5299,9 @@
       <c r="F111" s="2">
         <v>64696904</v>
       </c>
-      <c r="G111" s="2"/>
+      <c r="G111" s="2">
+        <v>0</v>
+      </c>
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
       <c r="J111">
@@ -5259,7 +5332,9 @@
       <c r="F112" s="2">
         <v>0</v>
       </c>
-      <c r="G112" s="2"/>
+      <c r="G112" s="2">
+        <v>0</v>
+      </c>
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
       <c r="J112">
@@ -5290,7 +5365,9 @@
       <c r="F113" s="2">
         <v>0</v>
       </c>
-      <c r="G113" s="2"/>
+      <c r="G113" s="2">
+        <v>0</v>
+      </c>
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
       <c r="J113">
@@ -5321,7 +5398,9 @@
       <c r="F114" s="2">
         <v>-725841475</v>
       </c>
-      <c r="G114" s="2"/>
+      <c r="G114" s="2">
+        <v>0</v>
+      </c>
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
       <c r="J114">
@@ -5352,7 +5431,9 @@
       <c r="F115" s="2">
         <v>362570806</v>
       </c>
-      <c r="G115" s="2"/>
+      <c r="G115" s="2">
+        <v>0</v>
+      </c>
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
       <c r="J115">
@@ -5383,7 +5464,9 @@
       <c r="F116" s="2">
         <v>815277317</v>
       </c>
-      <c r="G116" s="2"/>
+      <c r="G116" s="2">
+        <v>0</v>
+      </c>
       <c r="H116" s="2"/>
       <c r="I116" s="2"/>
       <c r="J116">
@@ -5414,7 +5497,9 @@
       <c r="F117" s="2">
         <v>61558431</v>
       </c>
-      <c r="G117" s="2"/>
+      <c r="G117" s="2">
+        <v>0</v>
+      </c>
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
       <c r="J117">
@@ -5445,7 +5530,9 @@
       <c r="F118" s="2">
         <v>18481352</v>
       </c>
-      <c r="G118" s="2"/>
+      <c r="G118" s="2">
+        <v>0</v>
+      </c>
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
       <c r="J118">
@@ -5476,7 +5563,9 @@
       <c r="F119" s="2">
         <v>0</v>
       </c>
-      <c r="G119" s="2"/>
+      <c r="G119" s="2">
+        <v>0</v>
+      </c>
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
       <c r="J119">
@@ -5507,7 +5596,9 @@
       <c r="F120" s="2">
         <v>4914996</v>
       </c>
-      <c r="G120" s="2"/>
+      <c r="G120" s="2">
+        <v>0</v>
+      </c>
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
       <c r="J120">
@@ -5538,7 +5629,9 @@
       <c r="F121" s="2">
         <v>3000000</v>
       </c>
-      <c r="G121" s="2"/>
+      <c r="G121" s="2">
+        <v>0</v>
+      </c>
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
       <c r="J121">
@@ -5569,7 +5662,9 @@
       <c r="F122" s="2">
         <v>0</v>
       </c>
-      <c r="G122" s="2"/>
+      <c r="G122" s="2">
+        <v>0</v>
+      </c>
       <c r="H122" s="2"/>
       <c r="I122" s="2"/>
       <c r="J122">
@@ -5600,7 +5695,9 @@
       <c r="F123" s="2">
         <v>66880810</v>
       </c>
-      <c r="G123" s="2"/>
+      <c r="G123" s="2">
+        <v>0</v>
+      </c>
       <c r="H123" s="2"/>
       <c r="I123" s="2"/>
       <c r="J123">
@@ -5631,7 +5728,9 @@
       <c r="F124" s="2">
         <v>223164508</v>
       </c>
-      <c r="G124" s="2"/>
+      <c r="G124" s="2">
+        <v>0</v>
+      </c>
       <c r="H124" s="2"/>
       <c r="I124" s="2"/>
       <c r="J124">
@@ -5662,7 +5761,9 @@
       <c r="F125" s="2">
         <v>22680000</v>
       </c>
-      <c r="G125" s="2"/>
+      <c r="G125" s="2">
+        <v>0</v>
+      </c>
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
       <c r="J125">
@@ -5693,7 +5794,9 @@
       <c r="F126" s="2">
         <v>29030767</v>
       </c>
-      <c r="G126" s="2"/>
+      <c r="G126" s="2">
+        <v>0</v>
+      </c>
       <c r="H126" s="2"/>
       <c r="I126" s="2"/>
       <c r="J126">
@@ -5724,7 +5827,9 @@
       <c r="F127" s="2">
         <v>32643059</v>
       </c>
-      <c r="G127" s="2"/>
+      <c r="G127" s="2">
+        <v>0</v>
+      </c>
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
       <c r="J127">
@@ -5755,7 +5860,9 @@
       <c r="F128" s="2">
         <v>79257186</v>
       </c>
-      <c r="G128" s="2"/>
+      <c r="G128" s="2">
+        <v>0</v>
+      </c>
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
       <c r="J128">
@@ -5786,7 +5893,9 @@
       <c r="F129" s="2">
         <v>61450000</v>
       </c>
-      <c r="G129" s="2"/>
+      <c r="G129" s="2">
+        <v>0</v>
+      </c>
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
       <c r="J129">
@@ -5814,7 +5923,9 @@
       </c>
       <c r="D130" s="2"/>
       <c r="E130" s="2"/>
-      <c r="F130" s="2"/>
+      <c r="F130" s="2">
+        <v>0</v>
+      </c>
       <c r="G130" s="2">
         <v>20915431</v>
       </c>
@@ -5845,7 +5956,9 @@
       </c>
       <c r="D131" s="2"/>
       <c r="E131" s="2"/>
-      <c r="F131" s="2"/>
+      <c r="F131" s="2">
+        <v>0</v>
+      </c>
       <c r="G131" s="2">
         <v>2690422</v>
       </c>
@@ -5876,7 +5989,9 @@
       </c>
       <c r="D132" s="2"/>
       <c r="E132" s="2"/>
-      <c r="F132" s="2"/>
+      <c r="F132" s="2">
+        <v>0</v>
+      </c>
       <c r="G132" s="2">
         <v>18225009</v>
       </c>
@@ -5910,7 +6025,9 @@
       <c r="F133" s="2">
         <v>46872777</v>
       </c>
-      <c r="G133" s="2"/>
+      <c r="G133" s="2">
+        <v>0</v>
+      </c>
       <c r="H133" s="2"/>
       <c r="I133" s="2"/>
       <c r="J133">
@@ -5941,7 +6058,9 @@
       <c r="F134" s="2">
         <v>46872777</v>
       </c>
-      <c r="G134" s="2"/>
+      <c r="G134" s="2">
+        <v>0</v>
+      </c>
       <c r="H134" s="2"/>
       <c r="I134" s="2"/>
       <c r="J134">

</xml_diff>